<commit_message>
creacion de hojas en el libro del excel
</commit_message>
<xml_diff>
--- a/excel/16-ejecicio-excel.xlsx
+++ b/excel/16-ejecicio-excel.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JesusCarvajal\Desktop\practicas\proyectos_pratica\evaluacion_cadean_tic\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8926024-F084-41D0-B6AE-6A630F7F43F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9012AB4-7F3B-43E0-99BC-43909625DEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Libro1" sheetId="1" r:id="rId1"/>
-    <sheet name="Libro2" sheetId="2" r:id="rId2"/>
+    <sheet name="pagina1" sheetId="2" r:id="rId1"/>
+    <sheet name="pagina2" sheetId="1" r:id="rId2"/>
+    <sheet name="pagina3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -346,24 +347,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C26" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D125FFAF-51C2-4F2D-A4DB-2E80353FE054}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -375,4 +358,34 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C26" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE10581E-E5D0-4545-A453-068842468C35}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
se borro una hoja del libro de excel
</commit_message>
<xml_diff>
--- a/excel/16-ejecicio-excel.xlsx
+++ b/excel/16-ejecicio-excel.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JesusCarvajal\Desktop\practicas\proyectos_pratica\evaluacion_cadean_tic\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9012AB4-7F3B-43E0-99BC-43909625DEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC57AE8-1F4F-449F-856C-B33F1E70A8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pagina1" sheetId="2" r:id="rId1"/>
     <sheet name="pagina2" sheetId="1" r:id="rId2"/>
-    <sheet name="pagina3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -364,8 +363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -376,16 +375,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE10581E-E5D0-4545-A453-068842468C35}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>